<commit_message>
Update data to support WKT2_2019
</commit_message>
<xml_diff>
--- a/data-raw/hrms.xlsx
+++ b/data-raw/hrms.xlsx
@@ -804,7 +804,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="R2" sqref="R2"/>
+      <selection pane="topRight" activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="15.25"/>
@@ -877,7 +877,7 @@
         <v>114</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1">
         <v>-63</v>
@@ -886,7 +886,7 @@
         <v>122</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J2" s="1">
         <v>-164</v>
@@ -918,7 +918,7 @@
         <v>114</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D3" s="1">
         <v>-78.099999999999994</v>
@@ -937,7 +937,7 @@
         <v>122</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J3" s="1">
         <v>-171.5</v>

</xml_diff>